<commit_message>
To prevent git stach from confusing us
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>aaromal</t>
+          <t>Aaromal</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>15:53:32</t>
+          <t>14:56:36</t>
         </is>
       </c>
     </row>

</xml_diff>